<commit_message>
Loading updata datasets from county.
</commit_message>
<xml_diff>
--- a/data/voting-places/20141104/20141104_G14_Webload_FINAL.xlsx
+++ b/data/voting-places/20141104/20141104_G14_Webload_FINAL.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EDay" sheetId="1" r:id="rId1"/>
     <sheet name="EV Perm" sheetId="2" r:id="rId2"/>
     <sheet name="Mobile" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EDay!$M$1:$M$187</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2446" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2446" uniqueCount="644">
   <si>
     <t>Pct.</t>
   </si>
@@ -1884,21 +1887,12 @@
     <t>0424</t>
   </si>
   <si>
-    <t>Del Valle ISD Admin Bldg.</t>
-  </si>
-  <si>
-    <t>5301 Ross Rd.</t>
-  </si>
-  <si>
     <t>0432</t>
   </si>
   <si>
     <t>0431</t>
   </si>
   <si>
-    <t>3909 North IH 35</t>
-  </si>
-  <si>
     <t>0602</t>
   </si>
   <si>
@@ -1911,9 +1905,6 @@
     <t>0802</t>
   </si>
   <si>
-    <t>Highland Mall</t>
-  </si>
-  <si>
     <t>0801</t>
   </si>
   <si>
@@ -1954,12 +1945,6 @@
   </si>
   <si>
     <t>9911 Brodie Lane</t>
-  </si>
-  <si>
-    <t>Randalls Research and Braker</t>
-  </si>
-  <si>
-    <t>Randalls South Mopac and William Cannon</t>
   </si>
   <si>
     <t>228, 267</t>
@@ -2839,8 +2824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="B175" sqref="B175:B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2848,7 +2833,7 @@
     <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="9" customWidth="1"/>
     <col min="4" max="4" width="41.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="9" customWidth="1"/>
     <col min="7" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="9" customWidth="1"/>
@@ -5780,7 +5765,7 @@
         <v>134</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>135</v>
@@ -6999,7 +6984,7 @@
         <v>180</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>181</v>
@@ -12773,7 +12758,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13019,10 +13004,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>622</v>
+        <v>331</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>623</v>
+        <v>332</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>333</v>
@@ -13046,7 +13031,7 @@
         <v>524</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="K7" s="17" t="s">
         <v>17</v>
@@ -13084,7 +13069,7 @@
         <v>432</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="K8" s="17" t="s">
         <v>17</v>
@@ -13098,7 +13083,7 @@
         <v>84</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>626</v>
+        <v>85</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>14</v>
@@ -13122,7 +13107,7 @@
         <v>432</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>17</v>
@@ -13160,7 +13145,7 @@
         <v>432</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>17</v>
@@ -13198,7 +13183,7 @@
         <v>432</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>17</v>
@@ -13236,7 +13221,7 @@
         <v>432</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>17</v>
@@ -13247,7 +13232,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>631</v>
+        <v>71</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>72</v>
@@ -13274,7 +13259,7 @@
         <v>524</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>17</v>
@@ -13312,7 +13297,7 @@
         <v>432</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>17</v>
@@ -13323,7 +13308,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -13349,7 +13334,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -13375,7 +13360,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -13401,7 +13386,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -13427,7 +13412,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -13453,7 +13438,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -13479,7 +13464,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -13505,7 +13490,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -13531,7 +13516,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -13595,7 +13580,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>409</v>
@@ -13633,10 +13618,10 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>14</v>
@@ -13747,7 +13732,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>646</v>
+        <v>235</v>
       </c>
       <c r="B29" s="17" t="s">
         <v>236</v>
@@ -13785,7 +13770,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>647</v>
+        <v>285</v>
       </c>
       <c r="B30" s="17" t="s">
         <v>286</v>
@@ -13870,7 +13855,7 @@
         <v>14</v>
       </c>
       <c r="D32" s="17">
-        <v>78713</v>
+        <v>78712</v>
       </c>
       <c r="E32" s="17">
         <v>30.286086000000001</v>
@@ -13907,8 +13892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14050,7 +14035,7 @@
         <v>218</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>527</v>
+        <v>219</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>14</v>

</xml_diff>